<commit_message>
Big success, veikia callas į generavimo funciją
</commit_message>
<xml_diff>
--- a/antife/rekomendacijos.xlsx
+++ b/antife/rekomendacijos.xlsx
@@ -699,7 +699,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Receptas: MORKŲ BLYNELIAI</t>
+          <t>Receptas: AVOKADŲ IR PESTO MAKARONŲ SALOTOS</t>
         </is>
       </c>
     </row>
@@ -711,7 +711,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Receptas: SALDŽIŲJŲ BULVIŲ SKILTELĖS</t>
+          <t>Produktas: Baklažanai</t>
         </is>
       </c>
     </row>
@@ -723,7 +723,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Produktas: Avižiniai dribsniai</t>
+          <t>Receptas: KREMINIAI GRYBŲ MAKARONAI</t>
         </is>
       </c>
     </row>
@@ -735,7 +735,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Receptas: KARŠTI IR RŪGŠTŪS BAKLAŽANAI</t>
+          <t>Produktas: Rabarbarai</t>
         </is>
       </c>
     </row>

</xml_diff>